<commit_message>
Work on extra decomp figures
</commit_message>
<xml_diff>
--- a/Replication Package/Code and Data/(3) Core Results/Decompositions/Output Data Python (New Model)/baseline.xlsx
+++ b/Replication Package/Code and Data/(3) Core Results/Decompositions/Output Data Python (New Model)/baseline.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:AH20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -553,6 +553,61 @@
           <t>magpty</t>
         </is>
       </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>wage_contr_to_ed</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>cu_contr_to_ed</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>ngdppot_contr_to_ed</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>wage_contr_shortage</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>cu_contr_shortage</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>ngdppot_contr_shortage</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>wage_contr_gcpi_via_ed</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>cu_contr_gcpi_via_ed</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>ngdppot_contr_gcpi_via_ed</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>gcu_contr_gcpi</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>gcu_contr_gw</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -624,6 +679,39 @@
       <c r="W2" t="n">
         <v>1.128416530824383</v>
       </c>
+      <c r="X2" t="n">
+        <v>-0.02922048654658926</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>-0.03428013632427085</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.03530281914597388</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -695,6 +783,39 @@
       <c r="W3" t="n">
         <v>1.512595805813133</v>
       </c>
+      <c r="X3" t="n">
+        <v>-0.02257103463570331</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>-0.02148138566120839</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0.02701215687793024</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -766,6 +887,39 @@
       <c r="W4" t="n">
         <v>1.871596231659467</v>
       </c>
+      <c r="X4" t="n">
+        <v>-0.01596550603039404</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>-0.01174630630727247</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.01658896895558648</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -837,6 +991,39 @@
       <c r="W5" t="n">
         <v>1.660541678943162</v>
       </c>
+      <c r="X5" t="n">
+        <v>-0.00722546496104215</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>-0.008013531667309337</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.008171313520501045</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -908,6 +1095,39 @@
       <c r="W6" t="n">
         <v>1.729278982489024</v>
       </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>-0</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -979,6 +1199,39 @@
       <c r="W7" t="n">
         <v>1.537662139982121</v>
       </c>
+      <c r="X7" t="n">
+        <v>0.01002873734811605</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0.01797784164150862</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>-0.009570804711598768</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>-0.4638241214031894</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>-0.8314662469114171</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0.4426449644044898</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>-0.04981026362410087</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>-0.08929150305487896</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0.04753582522221271</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>-0.005579484131193801</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>-0.01513906515331653</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -1050,6 +1303,39 @@
       <c r="W8" t="n">
         <v>3.336048444763229</v>
       </c>
+      <c r="X8" t="n">
+        <v>0.01358619396364347</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.151029665444864</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>-0.01080228479886713</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>-0.4494422820657746</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>-4.996183454970099</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0.3573483158358565</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>-0.04623461776667726</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>-0.5139628413931331</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>0.03676081101292281</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>0.02179755112064807</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>0.06700597961610644</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -1121,6 +1407,39 @@
       <c r="W9" t="n">
         <v>3.940007692958902</v>
       </c>
+      <c r="X9" t="n">
+        <v>0.01925193149932092</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0.0570863383509046</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>-0.02433943722991216</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>5.137671798238795</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>15.23436080273326</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>-6.495350362405663</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>0.5958176398652898</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>1.76673428253093</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>-0.7532681095653786</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>-0.002874316744263083</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>-0.03803185522194674</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -1192,6 +1511,39 @@
       <c r="W10" t="n">
         <v>3.574689640047302</v>
       </c>
+      <c r="X10" t="n">
+        <v>0.02769080014518543</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0.03380811693513852</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>-0.03596874897671043</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>-2.35185402389182</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>-2.871414167782195</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>3.05492244975591</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>-0.7673986580634803</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>-0.9369286344796877</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>0.996806504406806</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>0.6672117410865654</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>1.816429832215487</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -1263,6 +1615,39 @@
       <c r="W11" t="n">
         <v>3.577612786995887</v>
       </c>
+      <c r="X11" t="n">
+        <v>0.03952525779218874</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0.02560003899315788</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>-0.0534259920417739</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>-37.96857307754263</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>-24.59179283308175</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>51.32183308565772</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>-2.617753571642041</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>-1.695487828589405</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>3.538397705618817</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>-0.1480237479286686</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>-1.359058385987417</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -1334,6 +1719,39 @@
       <c r="W12" t="n">
         <v>3.5548188871807</v>
       </c>
+      <c r="X12" t="n">
+        <v>0.04779546344085972</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0.003527788320844216</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>-0.07372653861091294</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>-14.83048461656292</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>-1.09463967197447</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>22.87665435140111</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>-2.234846855327226</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>-0.1649542878657146</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>3.447346486610327</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>-0.1402262041891262</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>-0.2184911543699735</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -1405,6 +1823,39 @@
       <c r="W13" t="n">
         <v>2.891726937267691</v>
       </c>
+      <c r="X13" t="n">
+        <v>0.06345802400381562</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>-0.005226721957527047</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>-0.0937641366886055</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>-3.629623999308326</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0.298954084255937</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>5.363050081403819</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>1.252551093457823</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>-0.1031664065478445</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>-1.850741080897506</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>0.2238005034421153</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>0.3535042657350278</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -1476,6 +1927,39 @@
       <c r="W14" t="n">
         <v>2.972223430301435</v>
       </c>
+      <c r="X14" t="n">
+        <v>0.07621415534825271</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>-0.01592334306286691</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>-0.1162555345731047</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>4.337734590342479</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>-0.9062783111887008</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>-6.616692808996318</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>-0.1038825724622378</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>0.02170407625736768</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>0.1584603796924925</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>-0.2038707602638858</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>-0.4700099198750243</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -1547,6 +2031,39 @@
       <c r="W15" t="n">
         <v>2.250584675231826</v>
       </c>
+      <c r="X15" t="n">
+        <v>0.08880961520123165</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>-0.01922334998873865</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>-0.1417266661597019</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>0.5412848242629492</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>-0.1171642011602282</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>-0.8638084222277318</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>-0.3552937029762585</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>0.0769053574394144</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>0.5669948227594857</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>-0.1236228666022026</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>0.01198166855976179</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -1618,6 +2135,39 @@
       <c r="W16" t="n">
         <v>-0.219016638976699</v>
       </c>
+      <c r="X16" t="n">
+        <v>0.1031983526533304</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>-0.02303083280429785</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>-0.1696111612386186</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>-1.999661797231634</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>0.4462656169705559</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>3.286534627663119</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>0.325109545015457</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>-0.07255487497445724</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>-0.534332245060804</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>-0.01340588119028752</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>-0.06900073680243679</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -1689,6 +2239,39 @@
       <c r="W17" t="n">
         <v>-0.8560581919365262</v>
       </c>
+      <c r="X17" t="n">
+        <v>0.1148188836763495</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>-0.01999482553647258</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>-0.1863278053582871</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>1.233603995280957</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>-0.2148226483046615</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>-2.001889565220194</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>-0.0384957408619013</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>0.006703737205812268</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>0.06247079470532135</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>-0.1372600118236607</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>-0.08632726983346561</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -1760,6 +2343,39 @@
       <c r="W18" t="n">
         <v>-0.2096032942362047</v>
       </c>
+      <c r="X18" t="n">
+        <v>0.1263059276634806</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>-0.01104843406225964</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>-0.2011288848330306</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>1.857797933557207</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>-0.1625082713821334</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>-2.958347510158123</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>0.009788681531332758</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>-0.0008562512025843619</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>-0.01558744420632512</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>-0.06225814411308583</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>-0.02345471088259909</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -1831,6 +2447,39 @@
       <c r="W19" t="n">
         <v>-0.7746714240972175</v>
       </c>
+      <c r="X19" t="n">
+        <v>0.1382896724646008</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>-0.007793395941804171</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>-0.2157638358458023</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>-1.650681587438936</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>0.09302513308107292</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>2.575444606371685</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>-0.01760139856652062</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>0.0009919371831147647</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>0.02746224792697688</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>-0.0235713039910781</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>0.004103230162844973</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -1901,6 +2550,39 @@
       </c>
       <c r="W20" t="n">
         <v>-0.6383455064458143</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0.1482710404226308</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>-0.00466377738107937</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>-0.2259159112090003</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>0.06588312639778197</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>-0.002072314551870309</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>-0.1003840432428832</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>0.0201731748905018</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>-0.0006345352166593454</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>-0.03073723077936015</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>-0.01525976423996189</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>0.08987924439261885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>